<commit_message>
updates from testing matrix
</commit_message>
<xml_diff>
--- a/Ella_testing/siman testing matrix setup and analyse.xlsx
+++ b/Ella_testing/siman testing matrix setup and analyse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\siman\Ella_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB8C0EC-DF26-4A61-AC5F-23A730C6AE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAF7A18-3B50-4BA4-9461-E4E2F0BD289E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{72B21B36-5E99-47D1-84FC-B6B473904E03}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="23">
   <si>
     <t>* DGM defined by 1 variable:</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>N/A (wide label)</t>
+  </si>
+  <si>
+    <t>N/A (as target is in wide format)</t>
+  </si>
+  <si>
+    <t>N/A (becomes long-wide format)</t>
+  </si>
+  <si>
+    <t>N/A (becomes wide-long format)</t>
+  </si>
+  <si>
+    <t>N/A (becomes long-long format)</t>
   </si>
 </sst>
 </file>
@@ -460,18 +472,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA163D9-D4AD-40D9-85B9-98312487FF64}">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="54.1796875" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" customWidth="1"/>
     <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="25.90625" customWidth="1"/>
-    <col min="5" max="5" width="21.1796875" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" customWidth="1"/>
+    <col min="4" max="4" width="27.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -506,9 +516,15 @@
       <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -517,10 +533,18 @@
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -529,10 +553,18 @@
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -541,10 +573,18 @@
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -558,10 +598,18 @@
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -570,10 +618,18 @@
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
@@ -582,10 +638,18 @@
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -599,10 +663,18 @@
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -611,10 +683,18 @@
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -626,9 +706,15 @@
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
@@ -637,10 +723,18 @@
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -657,9 +751,15 @@
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -671,9 +771,15 @@
       <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
@@ -685,9 +791,15 @@
       <c r="C23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
@@ -696,10 +808,18 @@
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -713,10 +833,18 @@
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="C27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
@@ -728,9 +856,15 @@
       <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="D28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -739,10 +873,18 @@
       <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="C29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
@@ -751,10 +893,18 @@
       <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="C30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>